<commit_message>
A Unitary equation test of Tensorflow.
</commit_message>
<xml_diff>
--- a/PumpData/SFDC_API_Worklist.xlsx
+++ b/PumpData/SFDC_API_Worklist.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\da.long\PycharmProjects\test\PumpData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\da.long\PycharmProjects\Python-Learning-Code\PumpData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0F7DC6DE-3786-411C-B8CB-FD237A679365}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3B9129-B93B-4DEB-B3B3-08507A7EA175}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="96" windowWidth="16332" windowHeight="10836"/>
+    <workbookView xWindow="480" yWindow="96" windowWidth="16332" windowHeight="10836" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SFDC_API_Worklist" sheetId="1" r:id="rId1"/>
+    <sheet name="SFDC_API" sheetId="1" r:id="rId1"/>
+    <sheet name="SFDC_API_Get" sheetId="3" r:id="rId2"/>
+    <sheet name="SFDC_API_Post" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="83">
   <si>
     <t>API</t>
   </si>
@@ -168,13 +170,121 @@
   </si>
   <si>
     <t>C:\Users\da.long\source\Workspaces\MFP_Merck\MFP.WebAPI\Controllers\WeShare\WeShareController.cs</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.WindowsService.SFDC.DataFetch\FetchService.cs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		var r = service.GetAPI(</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\ToT\ToTService.cs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		string resultJson = this.GetAPI(</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Survey\SurveyService.cs</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Medical\MedicalService.cs</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\DSM\DSMService.cs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              string resultJson = this.GetAPI(</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Calendar\CallServicesSF.cs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	//string retString = this.GetAPI(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		string retString = this.GetAPI(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">			retString = this.GetAPI(</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Calendar\CallServicesRedis.cs</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Calendar\CalendarServicesSF.cs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">			string retString = this.GetAPI(</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Base\Service.cs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	string retString = this.GetAPI(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	string retString = this.PostAPI(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	//    string retString = this.PostAPI(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		string resultJson = this.PostAPI(</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Suggestion\SuggestionService.cs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          string retString = this.PostAPI(</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Runtime\LoginService.cs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		string retString = this.PostAPI(</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\NTHDoctor\NTHDoctorService.cs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          var sfdcResultJson = this.PostAPI(</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Cycle\CyclePlanService.cs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">			string resultJson = this.PostAPI(</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Calendar\ProdMessageRedis.cs</t>
+  </si>
+  <si>
+    <t>//    string retString = this.PostAPI(</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Calendar\POARedis.cs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	string sfdcResultJson = this.PostAPI(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          //string retString = this.PostAPI(</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Calendar\CallProdMessageServicesSF.cs</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Calendar\CallProdAccountServicesSF.cs</t>
+  </si>
+  <si>
+    <t>C:\Users\da.long\source\Workspaces\OCE Wechat Demo\MFP.Services\Calendar\CallPOAServicesSF.cs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -191,8 +301,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +317,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,11 +336,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -229,9 +351,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="1" xr:uid="{E4E52E9D-6EB8-4882-BBF0-E66191B62878}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -542,14 +671,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1173,4 +1302,736 @@
     <oddFooter>&amp;F</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778F6E1E-E13F-457E-B123-899AB2D855E1}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="5">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="5">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="5">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="5">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="5">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="5">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="5">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="5">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="5">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="5">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="5">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="5">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="5">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="5">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;P</oddHeader>
+    <oddFooter>&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4C674B-B547-4976-B595-62685437CB6B}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="5">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="5">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="5">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="5">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="5">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="5">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="5">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="5">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="5">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="5">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="5">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="5">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="5">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="5">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="5">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="5">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="5">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="5">
+        <v>481</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;P</oddHeader>
+    <oddFooter>&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>